<commit_message>
HW6: Finished Base Work
Troubleshooted work to get a reasonable output on the scatterplot. Needed to un-normalize the 2nd stage model prediction.
</commit_message>
<xml_diff>
--- a/hw/HW4-Similarity&LinearRegression/artifacts/BattingSalaries_1_DQR2.xlsx
+++ b/hw/HW4-Similarity&LinearRegression/artifacts/BattingSalaries_1_DQR2.xlsx
@@ -635,115 +635,115 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="D2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="E2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="F2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="G2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="H2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="I2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="J2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="K2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="L2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="M2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="N2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="O2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="P2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="Q2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="R2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="S2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="T2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="U2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="V2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="W2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="X2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="Y2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="Z2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AA2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AB2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AC2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AD2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AE2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AF2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AG2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AH2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AI2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AJ2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AK2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AL2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
       <c r="AM2" t="n">
-        <v>6080</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="3">
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
         <v>4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>5</v>
       </c>
       <c r="E3" t="n">
         <v>30</v>
@@ -768,100 +768,100 @@
         <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H3" t="n">
-        <v>632</v>
+        <v>400</v>
       </c>
       <c r="I3" t="n">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="J3" t="n">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="K3" t="n">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="L3" t="n">
+        <v>11</v>
+      </c>
+      <c r="M3" t="n">
+        <v>44</v>
+      </c>
+      <c r="N3" t="n">
+        <v>109</v>
+      </c>
+      <c r="O3" t="n">
+        <v>37</v>
+      </c>
+      <c r="P3" t="n">
         <v>14</v>
       </c>
-      <c r="M3" t="n">
-        <v>52</v>
-      </c>
-      <c r="N3" t="n">
-        <v>128</v>
-      </c>
-      <c r="O3" t="n">
-        <v>46</v>
-      </c>
-      <c r="P3" t="n">
-        <v>17</v>
-      </c>
       <c r="Q3" t="n">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="R3" t="n">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="S3" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="T3" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="U3" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="V3" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="W3" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="X3" t="n">
-        <v>1670</v>
+        <v>533</v>
       </c>
       <c r="Y3" t="n">
-        <v>1743</v>
+        <v>564</v>
       </c>
       <c r="Z3" t="n">
-        <v>1403</v>
+        <v>480</v>
       </c>
       <c r="AA3" t="n">
-        <v>842</v>
+        <v>297</v>
       </c>
       <c r="AB3" t="n">
-        <v>1384</v>
+        <v>444</v>
       </c>
       <c r="AC3" t="n">
-        <v>1714</v>
+        <v>539</v>
       </c>
       <c r="AD3" t="n">
-        <v>1102</v>
+        <v>344</v>
       </c>
       <c r="AE3" t="n">
-        <v>843</v>
+        <v>305</v>
       </c>
       <c r="AF3" t="n">
-        <v>1671</v>
+        <v>532</v>
       </c>
       <c r="AG3" t="n">
-        <v>2007</v>
+        <v>611</v>
       </c>
       <c r="AH3" t="n">
-        <v>809</v>
+        <v>269</v>
       </c>
       <c r="AI3" t="n">
-        <v>1104</v>
+        <v>381</v>
       </c>
       <c r="AJ3" t="n">
-        <v>735</v>
+        <v>289</v>
       </c>
       <c r="AK3" t="n">
-        <v>952</v>
+        <v>361</v>
       </c>
       <c r="AL3" t="n">
-        <v>1246</v>
+        <v>445</v>
       </c>
       <c r="AM3" t="n">
         <v>393</v>
@@ -877,10 +877,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2017.524342105263</v>
+        <v>2016</v>
       </c>
       <c r="D4" t="n">
-        <v>1.102138157894737</v>
+        <v>1.092380310182063</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -893,103 +893,103 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>46.7875</v>
+        <v>47.50573162508429</v>
       </c>
       <c r="H4" t="n">
-        <v>109.0807565789474</v>
+        <v>111.6392447741065</v>
       </c>
       <c r="I4" t="n">
-        <v>14.7077302631579</v>
+        <v>14.6621712744437</v>
       </c>
       <c r="J4" t="n">
-        <v>27.55723684210526</v>
+        <v>28.50708024275118</v>
       </c>
       <c r="K4" t="n">
-        <v>5.500986842105263</v>
+        <v>5.565745111260958</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5427631578947368</v>
+        <v>0.588671611598112</v>
       </c>
       <c r="M4" t="n">
-        <v>3.959868421052632</v>
+        <v>3.782872555630479</v>
       </c>
       <c r="N4" t="n">
-        <v>14.04276315789474</v>
+        <v>13.98853674983142</v>
       </c>
       <c r="O4" t="n">
-        <v>1.614802631578947</v>
+        <v>1.710721510451787</v>
       </c>
       <c r="P4" t="n">
-        <v>0.6126644736842105</v>
+        <v>0.6749831422791639</v>
       </c>
       <c r="Q4" t="n">
-        <v>10.27927631578947</v>
+        <v>10.17397167902899</v>
       </c>
       <c r="R4" t="n">
-        <v>26.82828947368421</v>
+        <v>26.28590694538098</v>
       </c>
       <c r="S4" t="n">
-        <v>0.5894736842105263</v>
+        <v>0.6284558327714093</v>
       </c>
       <c r="T4" t="n">
-        <v>1.203947368421053</v>
+        <v>1.113283884018881</v>
       </c>
       <c r="U4" t="n">
-        <v>0.5837171052631579</v>
+        <v>0.6911665542818611</v>
       </c>
       <c r="V4" t="n">
-        <v>0.7840460526315789</v>
+        <v>0.8186109238031019</v>
       </c>
       <c r="W4" t="n">
-        <v>2.375493421052632</v>
+        <v>2.507754551584626</v>
       </c>
       <c r="X4" t="n">
-        <v>0.3846753997063246</v>
+        <v>0.3778254854598996</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.1274012683404958</v>
+        <v>0.1292882898205744</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.02368218502183766</v>
+        <v>0.02410559533737742</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.002242200995212711</v>
+        <v>0.002443420874401912</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.01437704739068628</v>
+        <v>0.01359440458305515</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.3778238989917216</v>
+        <v>0.05783632124471515</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.3241436011247175</v>
+        <v>0.3191713036101222</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.003032659696875451</v>
+        <v>0.004077921723339313</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.3671846299672112</v>
+        <v>0.3564420767356366</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.2410062015126544</v>
+        <v>0.2337153418023637</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.001921721791647101</v>
+        <v>0.001977483714266949</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.005569989730624332</v>
+        <v>0.005052931276727442</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.336676692976459</v>
+        <v>0.3338294163315963</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.003805775965506785</v>
+        <v>0.003499109577459762</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.01342657664587985</v>
+        <v>0.01322318488256458</v>
       </c>
       <c r="AM4" t="n">
-        <v>2113826.670888158</v>
+        <v>3396605.636547539</v>
       </c>
     </row>
     <row r="5">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -1018,10 +1018,10 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -1069,10 +1069,10 @@
         <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>0.1396578764999818</v>
+        <v>0.1352657004830918</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.1052631578947368</v>
+        <v>0.1219512195121951</v>
       </c>
       <c r="Z5" t="n">
         <v>0</v>
@@ -1084,19 +1084,19 @@
         <v>0</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1328952192008281</v>
+        <v>0</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.009009038256759213</v>
+        <v>0.008976660682226212</v>
       </c>
       <c r="AE5" t="n">
         <v>0</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.101898810239154</v>
+        <v>0.09565217391304348</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.216</v>
+        <v>0.2042253521126761</v>
       </c>
       <c r="AH5" t="n">
         <v>0</v>
@@ -1105,7 +1105,7 @@
         <v>0</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.005031454501727782</v>
+        <v>0.00816326530612245</v>
       </c>
       <c r="AK5" t="n">
         <v>0</v>
@@ -1127,10 +1127,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1535</v>
+        <v>1483</v>
       </c>
       <c r="D6" t="n">
-        <v>5500</v>
+        <v>1353</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1143,113 +1143,103 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="H6" t="n">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="I6" t="n">
-        <v>371</v>
+        <v>95</v>
       </c>
       <c r="J6" t="n">
-        <v>345</v>
+        <v>83</v>
       </c>
       <c r="K6" t="n">
-        <v>3463</v>
+        <v>831</v>
       </c>
       <c r="L6" t="n">
-        <v>4727</v>
+        <v>1141</v>
       </c>
       <c r="M6" t="n">
-        <v>3830</v>
+        <v>941</v>
       </c>
       <c r="N6" t="n">
-        <v>3178</v>
+        <v>765</v>
       </c>
       <c r="O6" t="n">
-        <v>4451</v>
+        <v>1087</v>
       </c>
       <c r="P6" t="n">
-        <v>4713</v>
+        <v>1136</v>
       </c>
       <c r="Q6" t="n">
-        <v>3179</v>
+        <v>771</v>
       </c>
       <c r="R6" t="n">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="S6" t="n">
-        <v>4883</v>
+        <v>1181</v>
       </c>
       <c r="T6" t="n">
-        <v>4226</v>
+        <v>1038</v>
       </c>
       <c r="U6" t="n">
-        <v>4655</v>
+        <v>1083</v>
       </c>
       <c r="V6" t="n">
-        <v>4351</v>
+        <v>1059</v>
       </c>
       <c r="W6" t="n">
-        <v>3693</v>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+        <v>886</v>
+      </c>
+      <c r="X6" t="n">
+        <v>1</v>
       </c>
       <c r="Y6" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Z6" t="n">
-        <v>3463</v>
+        <v>831</v>
       </c>
       <c r="AA6" t="n">
-        <v>4727</v>
+        <v>1141</v>
       </c>
       <c r="AB6" t="n">
-        <v>3830</v>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+        <v>941</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>765</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>1</v>
       </c>
       <c r="AE6" t="n">
-        <v>4713</v>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+        <v>1136</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>1</v>
       </c>
       <c r="AG6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH6" t="n">
-        <v>4883</v>
+        <v>1181</v>
       </c>
       <c r="AI6" t="n">
-        <v>4226</v>
-      </c>
-      <c r="AJ6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+        <v>1038</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>1</v>
       </c>
       <c r="AK6" t="n">
-        <v>4351</v>
+        <v>1059</v>
       </c>
       <c r="AL6" t="n">
-        <v>3693</v>
+        <v>886</v>
       </c>
       <c r="AM6" t="n">
-        <v>5181</v>
+        <v>584</v>
       </c>
     </row>
     <row r="7">
@@ -1262,7 +1252,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -1278,7 +1268,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1344,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="AC7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -1387,10 +1377,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1568</v>
+        <v>1483</v>
       </c>
       <c r="D8" t="n">
-        <v>5500</v>
+        <v>1353</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1403,103 +1393,103 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>164</v>
+        <v>36</v>
       </c>
       <c r="H8" t="n">
-        <v>1926</v>
+        <v>460</v>
       </c>
       <c r="I8" t="n">
-        <v>3034</v>
+        <v>722</v>
       </c>
       <c r="J8" t="n">
-        <v>2786</v>
+        <v>669</v>
       </c>
       <c r="K8" t="n">
-        <v>3463</v>
+        <v>831</v>
       </c>
       <c r="L8" t="n">
-        <v>4727</v>
+        <v>1141</v>
       </c>
       <c r="M8" t="n">
-        <v>3830</v>
+        <v>941</v>
       </c>
       <c r="N8" t="n">
-        <v>3178</v>
+        <v>765</v>
       </c>
       <c r="O8" t="n">
-        <v>4451</v>
+        <v>1087</v>
       </c>
       <c r="P8" t="n">
-        <v>4713</v>
+        <v>1136</v>
       </c>
       <c r="Q8" t="n">
-        <v>3179</v>
+        <v>771</v>
       </c>
       <c r="R8" t="n">
-        <v>2184</v>
+        <v>516</v>
       </c>
       <c r="S8" t="n">
-        <v>4883</v>
+        <v>1181</v>
       </c>
       <c r="T8" t="n">
-        <v>4226</v>
+        <v>1038</v>
       </c>
       <c r="U8" t="n">
-        <v>4655</v>
+        <v>1083</v>
       </c>
       <c r="V8" t="n">
-        <v>4351</v>
+        <v>1059</v>
       </c>
       <c r="W8" t="n">
-        <v>3693</v>
+        <v>886</v>
       </c>
       <c r="X8" t="n">
-        <v>1952</v>
+        <v>466</v>
       </c>
       <c r="Y8" t="n">
-        <v>2786</v>
+        <v>669</v>
       </c>
       <c r="Z8" t="n">
-        <v>3463</v>
+        <v>831</v>
       </c>
       <c r="AA8" t="n">
-        <v>4727</v>
+        <v>1141</v>
       </c>
       <c r="AB8" t="n">
-        <v>3830</v>
+        <v>941</v>
       </c>
       <c r="AC8" t="n">
-        <v>1942</v>
+        <v>765</v>
       </c>
       <c r="AD8" t="n">
-        <v>2525</v>
+        <v>627</v>
       </c>
       <c r="AE8" t="n">
-        <v>4713</v>
+        <v>1136</v>
       </c>
       <c r="AF8" t="n">
-        <v>1950</v>
+        <v>462</v>
       </c>
       <c r="AG8" t="n">
-        <v>2184</v>
+        <v>516</v>
       </c>
       <c r="AH8" t="n">
-        <v>4883</v>
+        <v>1181</v>
       </c>
       <c r="AI8" t="n">
-        <v>4226</v>
+        <v>1038</v>
       </c>
       <c r="AJ8" t="n">
-        <v>2750</v>
+        <v>630</v>
       </c>
       <c r="AK8" t="n">
-        <v>4351</v>
+        <v>1059</v>
       </c>
       <c r="AL8" t="n">
-        <v>3693</v>
+        <v>886</v>
       </c>
       <c r="AM8" t="n">
-        <v>5181</v>
+        <v>584</v>
       </c>
     </row>
     <row r="9">
@@ -1512,10 +1502,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.119478452963385</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3268869963723395</v>
+        <v>0.3077320038129833</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1528,103 +1518,103 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>44.53432435102395</v>
+        <v>45.32907642513199</v>
       </c>
       <c r="H9" t="n">
-        <v>173.9128823044439</v>
+        <v>177.9291053453142</v>
       </c>
       <c r="I9" t="n">
-        <v>25.84020783501953</v>
+        <v>25.80268411024679</v>
       </c>
       <c r="J9" t="n">
-        <v>47.02172496954491</v>
+        <v>48.61975265205488</v>
       </c>
       <c r="K9" t="n">
-        <v>9.765939801529486</v>
+        <v>9.814760010817414</v>
       </c>
       <c r="L9" t="n">
-        <v>1.358375987372714</v>
+        <v>1.444681642891701</v>
       </c>
       <c r="M9" t="n">
-        <v>8.040285635880929</v>
+        <v>7.863978801666413</v>
       </c>
       <c r="N9" t="n">
-        <v>25.24486068258638</v>
+        <v>25.42524706553083</v>
       </c>
       <c r="O9" t="n">
-        <v>4.698578039353996</v>
+        <v>5.094312904896844</v>
       </c>
       <c r="P9" t="n">
-        <v>1.560367470118487</v>
+        <v>1.697688727030272</v>
       </c>
       <c r="Q9" t="n">
-        <v>18.93174287035385</v>
+        <v>18.66403578144393</v>
       </c>
       <c r="R9" t="n">
-        <v>41.38636067011032</v>
+        <v>40.84710948413129</v>
       </c>
       <c r="S9" t="n">
-        <v>1.803258110137459</v>
+        <v>1.857668056970902</v>
       </c>
       <c r="T9" t="n">
-        <v>2.696927426937631</v>
+        <v>2.498443281517798</v>
       </c>
       <c r="U9" t="n">
-        <v>1.468504010612805</v>
+        <v>1.565173064521483</v>
       </c>
       <c r="V9" t="n">
-        <v>1.636655120884894</v>
+        <v>1.69109087649545</v>
       </c>
       <c r="W9" t="n">
-        <v>4.364494856356894</v>
+        <v>4.600553040059128</v>
       </c>
       <c r="X9" t="n">
-        <v>0.4278975610061647</v>
+        <v>0.4257468807024696</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.1414893714632591</v>
+        <v>0.1373271511276778</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.04380579155251292</v>
+        <v>0.04394085827308228</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.007663163733927798</v>
+        <v>0.007626517667080745</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.02549071585247502</v>
+        <v>0.02713584014058783</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.4311361335839803</v>
+        <v>0.07664531078664973</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.461729238495197</v>
+        <v>0.4598706238918917</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.01871412488949996</v>
+        <v>0.02879855385072225</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.4386099075979086</v>
+        <v>0.4365026176660978</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.2589720949503738</v>
+        <v>0.2515131552269483</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.006042904641263938</v>
+        <v>0.005729023044261746</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.01953857531858745</v>
+        <v>0.01409937687392615</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.4595416652472252</v>
+        <v>0.4561314359548418</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.0221362164234495</v>
+        <v>0.01096076583240338</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.04448348870222812</v>
+        <v>0.04275229409667387</v>
       </c>
       <c r="AM9" t="n">
-        <v>2450397.585104827</v>
+        <v>4738327.13204564</v>
       </c>
     </row>
     <row r="10">
@@ -1762,10 +1752,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1781,22 +1771,22 @@
         <v>162</v>
       </c>
       <c r="H11" t="n">
-        <v>681</v>
+        <v>672</v>
       </c>
       <c r="I11" t="n">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="J11" t="n">
         <v>216</v>
       </c>
       <c r="K11" t="n">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="L11" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M11" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="N11" t="n">
         <v>133</v>
@@ -1808,19 +1798,19 @@
         <v>18</v>
       </c>
       <c r="Q11" t="n">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="R11" t="n">
         <v>219</v>
       </c>
       <c r="S11" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="T11" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="U11" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V11" t="n">
         <v>15</v>
@@ -1838,7 +1828,7 @@
         <v>1</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.25</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="AB11" t="n">
         <v>0.3333333333333333</v>
@@ -1859,16 +1849,16 @@
         <v>1</v>
       </c>
       <c r="AH11" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="AI11" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="AJ11" t="n">
         <v>1</v>
       </c>
       <c r="AK11" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="AL11" t="n">
         <v>1</v>
@@ -1897,10 +1887,10 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>235</v>
+        <v>60</v>
       </c>
       <c r="F12" t="n">
-        <v>3086</v>
+        <v>749</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1908,97 +1898,97 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>1926</v>
+        <v>460</v>
       </c>
       <c r="I12" t="n">
-        <v>3034</v>
+        <v>722</v>
       </c>
       <c r="J12" t="n">
-        <v>2786</v>
+        <v>669</v>
       </c>
       <c r="K12" t="n">
-        <v>3463</v>
+        <v>831</v>
       </c>
       <c r="L12" t="n">
-        <v>4727</v>
+        <v>1141</v>
       </c>
       <c r="M12" t="n">
-        <v>3830</v>
+        <v>941</v>
       </c>
       <c r="N12" t="n">
-        <v>3178</v>
+        <v>765</v>
       </c>
       <c r="O12" t="n">
-        <v>4451</v>
+        <v>1087</v>
       </c>
       <c r="P12" t="n">
-        <v>4713</v>
+        <v>1136</v>
       </c>
       <c r="Q12" t="n">
-        <v>3179</v>
+        <v>771</v>
       </c>
       <c r="R12" t="n">
-        <v>2184</v>
+        <v>516</v>
       </c>
       <c r="S12" t="n">
-        <v>4883</v>
+        <v>1181</v>
       </c>
       <c r="T12" t="n">
-        <v>4226</v>
+        <v>1038</v>
       </c>
       <c r="U12" t="n">
-        <v>4655</v>
+        <v>1083</v>
       </c>
       <c r="V12" t="n">
-        <v>4351</v>
+        <v>1059</v>
       </c>
       <c r="W12" t="n">
-        <v>3693</v>
+        <v>886</v>
       </c>
       <c r="X12" t="n">
-        <v>1114</v>
+        <v>265</v>
       </c>
       <c r="Y12" t="n">
-        <v>2786</v>
+        <v>669</v>
       </c>
       <c r="Z12" t="n">
-        <v>3463</v>
+        <v>831</v>
       </c>
       <c r="AA12" t="n">
-        <v>4727</v>
+        <v>1141</v>
       </c>
       <c r="AB12" t="n">
-        <v>3830</v>
+        <v>941</v>
       </c>
       <c r="AC12" t="n">
-        <v>1252</v>
+        <v>765</v>
       </c>
       <c r="AD12" t="n">
-        <v>2525</v>
+        <v>627</v>
       </c>
       <c r="AE12" t="n">
-        <v>4713</v>
+        <v>1136</v>
       </c>
       <c r="AF12" t="n">
-        <v>1264</v>
+        <v>315</v>
       </c>
       <c r="AG12" t="n">
-        <v>2184</v>
+        <v>516</v>
       </c>
       <c r="AH12" t="n">
-        <v>4883</v>
+        <v>1181</v>
       </c>
       <c r="AI12" t="n">
-        <v>4226</v>
+        <v>1038</v>
       </c>
       <c r="AJ12" t="n">
-        <v>2750</v>
+        <v>630</v>
       </c>
       <c r="AK12" t="n">
-        <v>4351</v>
+        <v>1059</v>
       </c>
       <c r="AL12" t="n">
-        <v>3693</v>
+        <v>886</v>
       </c>
       <c r="AM12" t="inlineStr">
         <is>

</xml_diff>